<commit_message>
EPBDS-14830 Improve logic for potentially indexed conditions with static left statement
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-14830.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-14830.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\bugs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vpikus/Sources/OpenL/openl-tablets/STUDIO/org.openl.rules.test/test-resources/functionality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD06B60C-7F85-4A05-9D31-9462581A4126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AEA49D-C71D-9644-BF80-4A09D64A2612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2CA8817B-84E3-4D5F-876C-05382B9F78EC}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="35040" windowHeight="21120" activeTab="1" xr2:uid="{2CA8817B-84E3-4D5F-876C-05382B9F78EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>C1</t>
   </si>
   <si>
-    <t>productType == "VPS" or assumedParticipationPct &lt; 0.5</t>
-  </si>
-  <si>
     <t>Boolean vpsOrLowParticipation</t>
   </si>
   <si>
@@ -53,37 +51,12 @@
     <t>Yes</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Rules Double </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">PreExConditionLimitationFactor </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Franklin Gothic Book"/>
-        <family val="2"/>
-      </rPr>
-      <t>(String productType, Double assumedParticipationPct)</t>
-    </r>
-  </si>
-  <si>
     <t>RET1</t>
   </si>
   <si>
     <t>Rules Double PreExConditionLimitationFactor (Boolean a, Boolean b)</t>
   </si>
   <si>
-    <t>a orb</t>
-  </si>
-  <si>
     <t>a or b</t>
   </si>
   <si>
@@ -111,7 +84,67 @@
     <t>_res_</t>
   </si>
   <si>
+    <t>Rules Double theRule(Integer a)</t>
+  </si>
+  <si>
+    <t>a==0 or isEmpty(a)</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Boolean Condition</t>
+  </si>
+  <si>
+    <t>Test theRule</t>
+  </si>
+  <si>
+    <t>_description_</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t>Rules Double myRule2(String a, String b, String c)</t>
+  </si>
+  <si>
+    <t>a== b or a== c</t>
+  </si>
+  <si>
+    <t>The codes</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test myRule2 </t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Rules Double myRule3(String a)</t>
+  </si>
+  <si>
+    <t>a== "test" or a== "bla"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test myRule3 </t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -119,12 +152,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,23 +170,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Franklin Gothic Book"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Franklin Gothic Book"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
@@ -168,18 +184,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" rgb="FFFFFF"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442" rgb="4EA72E"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -211,18 +227,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <right style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -234,74 +241,39 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1"/>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,134 +609,447 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2C6458-1D1F-40CB-ADE4-889EE5341D5E}">
-  <dimension ref="B11:H35"/>
+  <dimension ref="B11:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="43.7109375"/>
+    <col min="7" max="7" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="7:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G11" s="8" t="s">
+    <row r="11" spans="7:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="7:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="G13" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G15" s="1" t="s">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="C31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16" t="n" s="3">
+      <c r="C32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1.0049999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>0.99</v>
       </c>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17" t="s" s="2">
-        <v>4</v>
-      </c>
-      <c r="H17" t="n" s="3">
-        <v>1.005</v>
-      </c>
-    </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="7:10" x14ac:dyDescent="0.25"/>
-    <row r="30">
-      <c r="B30" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31">
-      <c r="B31" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s" s="12">
-        <v>15</v>
-      </c>
-      <c r="D31" t="s" s="12">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="s" s="12">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s" s="12">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s" s="12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C33" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33" s="12" t="n">
-        <v>1.005</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C34" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="12" t="n">
-        <v>1.005</v>
-      </c>
-    </row>
-    <row r="35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4FEA50-1403-3C45-B939-770435EEFFB9}">
+  <dimension ref="B2:E55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="D30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="8"/>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="D49" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D50" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" s="6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B52:C52"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>